<commit_message>
Add chart combining both forms of SD3
</commit_message>
<xml_diff>
--- a/data/investigate_sd3.xlsx
+++ b/data/investigate_sd3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\WCA\ons-stats\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0165F0AD-90F5-448C-A88C-8A147B777079}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{163FB892-7056-4D13-AADD-EF482DD28F6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="2" activeTab="7" xr2:uid="{BACCE0E3-7F96-4AD2-A101-44AECFFFC852}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="1" activeTab="8" xr2:uid="{BACCE0E3-7F96-4AD2-A101-44AECFFFC852}"/>
   </bookViews>
   <sheets>
     <sheet name="daily_phe" sheetId="6" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="frankenstein" sheetId="8" r:id="rId6"/>
     <sheet name="daily_limits" sheetId="4" r:id="rId7"/>
     <sheet name="weekly_limits" sheetId="5" r:id="rId8"/>
+    <sheet name="sd3_comparison" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
   <si>
     <t>DIFF</t>
   </si>
@@ -96,6 +97,12 @@
   <si>
     <t>England Weekly Deaths (ONS approx)</t>
   </si>
+  <si>
+    <t>incorrect lower bound</t>
+  </si>
+  <si>
+    <t>incorrect upper bound</t>
+  </si>
 </sst>
 </file>
 
@@ -103,8 +110,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="171" formatCode="0.000"/>
-    <numFmt numFmtId="172" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -159,8 +166,8 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -2710,7 +2717,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>lower bound</c:v>
+                  <c:v>incorrect lower bound</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3071,7 +3078,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>upper bound</c:v>
+                  <c:v>incorrect upper bound</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5399,6 +5406,2157 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>All cause deaths for England and Wales 2020</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>CONTRASTING the effect of different 3SD derivations</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>(Upper and lower bounds derived from Weekly Figures)</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>i.e. mean +/- weekly 3SD</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>pivoted!$A$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>E+W Weekly Deaths (ONS estimate)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>pivoted!$B$2:$BA$2</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="52"/>
+                <c:pt idx="0">
+                  <c:v>43833</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43840</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43847</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43854</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43861</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43868</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43875</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43882</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43889</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43896</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43903</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>43910</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43917</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>43924</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>43931</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>43938</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>43945</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>43952</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>43959</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>43966</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>43973</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>43980</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43987</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>43994</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>44001</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>44008</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>44015</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>44022</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>44029</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>44036</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>44043</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>44050</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>44057</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>44064</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>44071</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>44078</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>44085</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>44092</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>44099</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>44106</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>44113</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>44120</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>44127</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44134</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>44141</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>44148</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>44155</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>44162</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>44169</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>44176</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>44183</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>44190</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>pivoted!$B$23:$BB$23</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="53"/>
+                <c:pt idx="0">
+                  <c:v>12431</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12139</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11746</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10914</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11094</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10710</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10877</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10795</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10647</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10984</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10834</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11401</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13787</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>17897</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>22038</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>20922</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>18694</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>15825</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>13712</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>11948</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>11354</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>10220</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>9975</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9462</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>9220</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9671</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>8746</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>8682</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>8907</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>9090</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>8874</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>9009</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>10153</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>8840</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8675</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>9061</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>9140</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>9460</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>9605</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>9990</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>10351</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>10386</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>11092</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>11442</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>11781</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>12446</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>12566</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C135-4B1C-A3DE-3E0E7A411B98}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>pivoted!$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>baseline</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>pivoted!$B$2:$BA$2</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="52"/>
+                <c:pt idx="0">
+                  <c:v>43833</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43840</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43847</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43854</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43861</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43868</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43875</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43882</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43889</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43896</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43903</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>43910</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43917</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>43924</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>43931</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>43938</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>43945</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>43952</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>43959</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>43966</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>43973</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>43980</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43987</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>43994</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>44001</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>44008</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>44015</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>44022</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>44029</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>44036</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>44043</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>44050</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>44057</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>44064</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>44071</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>44078</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>44085</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>44092</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>44099</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>44106</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>44113</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>44120</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>44127</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44134</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>44141</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>44148</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>44155</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>44162</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>44169</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>44176</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>44183</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>44190</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>pivoted!$B$10:$BB$10</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="53"/>
+                <c:pt idx="0">
+                  <c:v>12700.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12895</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12618.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12173.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12079.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11670.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11660.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11402.4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11323.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11252.8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10910</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10607.2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10448.799999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10360.4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>10263.4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10084.799999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9812.2000000000007</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9743.7999999999993</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9746</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9537</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9500.2000000000007</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9197</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>9223.4</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9205.6</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>9275</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9051.6</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>9271.6</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>8903</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>9113.4</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>9125.7999999999993</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>8783.6</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>9050</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>9013.7999999999993</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>8974.7999999999993</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8939.2000000000007</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>8922.2000000000007</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>9132.6</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>9204</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>9450.4</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>9530.2000000000007</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>9812</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>9843.7999999999993</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>9823</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>10082.200000000001</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>10192.200000000001</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>10227.200000000001</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>10296.4</c:v>
+                </c:pt>
+                <c:pt idx="47" formatCode="General">
+                  <c:v>10467.6</c:v>
+                </c:pt>
+                <c:pt idx="48" formatCode="General">
+                  <c:v>10857.2</c:v>
+                </c:pt>
+                <c:pt idx="49" formatCode="General">
+                  <c:v>11032</c:v>
+                </c:pt>
+                <c:pt idx="50" formatCode="General">
+                  <c:v>11396.8</c:v>
+                </c:pt>
+                <c:pt idx="51" formatCode="General">
+                  <c:v>11616</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-C135-4B1C-A3DE-3E0E7A411B98}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>pivoted!$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>lower bound</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>pivoted!$B$2:$BA$2</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="52"/>
+                <c:pt idx="0">
+                  <c:v>43833</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43840</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43847</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43854</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43861</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43868</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43875</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43882</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43889</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43896</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43903</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>43910</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43917</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>43924</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>43931</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>43938</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>43945</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>43952</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>43959</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>43966</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>43973</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>43980</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43987</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>43994</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>44001</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>44008</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>44015</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>44022</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>44029</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>44036</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>44043</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>44050</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>44057</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>44064</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>44071</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>44078</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>44085</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>44092</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>44099</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>44106</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>44113</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>44120</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>44127</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44134</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>44141</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>44148</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>44155</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>44162</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>44169</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>44176</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>44183</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>44190</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>pivoted!$B$11:$BB$11</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="53"/>
+                <c:pt idx="0">
+                  <c:v>8538.0867999999991</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8859.8883000000005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9487.9120000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9766.1206000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10183.6754</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10741.7268</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10312.0226</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10287.0476</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9681.7263000000003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8645.9298999999992</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8646.4256999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8834.4945000000007</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8910.5640000000003</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9045.2188999999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9289.3917000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9012.3541000000005</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9069.3176000000003</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9446.6067000000003</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9135.9707999999991</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9131.6023999999998</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8612.6898999999994</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>8823.0262000000002</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>8387.6566000000003</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>8865.0313999999998</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>8146.2088000000003</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8409.7553000000007</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>8917.8055000000004</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>8380.7034999999996</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7724.7446</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>7841.0384999999997</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>8437.9010999999991</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>8786.0545999999995</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>8084.2677000000003</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>8504.6916999999994</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8182.7420000000002</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>8445.2682999999997</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>8829.2491000000009</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>8335.9698000000008</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>8700.8906999999999</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>9071.5064000000002</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>9390.7932000000001</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>8966.1036000000004</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>9066.3883000000005</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>9625.5949000000001</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>9386.9307000000008</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>9003.7245000000003</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>8748.8808000000008</c:v>
+                </c:pt>
+                <c:pt idx="47" formatCode="General">
+                  <c:v>9592.7255000000005</c:v>
+                </c:pt>
+                <c:pt idx="48" formatCode="General">
+                  <c:v>9675.4673999999995</c:v>
+                </c:pt>
+                <c:pt idx="49" formatCode="General">
+                  <c:v>9200.7934999999998</c:v>
+                </c:pt>
+                <c:pt idx="50" formatCode="General">
+                  <c:v>8975.6031000000003</c:v>
+                </c:pt>
+                <c:pt idx="51" formatCode="General">
+                  <c:v>8860.8042000000005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-C135-4B1C-A3DE-3E0E7A411B98}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>pivoted!$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>upper bound</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>pivoted!$B$2:$BA$2</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="52"/>
+                <c:pt idx="0">
+                  <c:v>43833</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43840</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43847</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43854</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43861</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43868</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43875</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43882</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43889</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43896</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43903</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>43910</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43917</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>43924</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>43931</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>43938</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>43945</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>43952</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>43959</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>43966</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>43973</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>43980</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43987</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>43994</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>44001</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>44008</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>44015</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>44022</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>44029</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>44036</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>44043</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>44050</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>44057</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>44064</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>44071</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>44078</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>44085</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>44092</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>44099</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>44106</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>44113</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>44120</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>44127</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44134</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>44141</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>44148</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>44155</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>44162</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>44169</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>44176</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>44183</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>44190</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>pivoted!$B$12:$BB$12</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="53"/>
+                <c:pt idx="0">
+                  <c:v>16862.713199999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16930.111700000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15749.288</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14580.679400000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13975.524600000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12599.8732</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13009.1774</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12517.752399999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12964.673699999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13859.670099999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13173.5743</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12379.905500000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11987.036</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>11675.581099999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>11237.408299999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11157.2459</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>10555.082399999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>10040.9933</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>10356.029200000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9942.3976000000002</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>10387.7101</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9570.9737999999998</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>10059.143400000001</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9546.1686000000009</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>10403.7912</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9693.4447</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>9625.3945000000003</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>9425.2965000000004</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>10502.055399999999</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>10410.5615</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>9129.2988999999998</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>9313.9454000000005</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>9943.3323</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>9444.9082999999991</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>9695.6579999999994</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>9399.1316999999999</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>9435.9508999999998</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>10072.030199999999</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>10199.909299999999</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>9988.8935999999994</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>10233.2068</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>10721.4964</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>10579.611699999999</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>10538.8051</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>10997.469300000001</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>11450.675499999999</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>11843.9192</c:v>
+                </c:pt>
+                <c:pt idx="47" formatCode="General">
+                  <c:v>11342.4745</c:v>
+                </c:pt>
+                <c:pt idx="48" formatCode="General">
+                  <c:v>12038.9326</c:v>
+                </c:pt>
+                <c:pt idx="49" formatCode="General">
+                  <c:v>12863.2065</c:v>
+                </c:pt>
+                <c:pt idx="50" formatCode="General">
+                  <c:v>13817.9969</c:v>
+                </c:pt>
+                <c:pt idx="51" formatCode="General">
+                  <c:v>14371.1958</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-C135-4B1C-A3DE-3E0E7A411B98}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>pivoted!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>incorrect lower bound</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>pivoted!$B$6:$BA$6</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="52"/>
+                <c:pt idx="1">
+                  <c:v>8691.5386999999992</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9298.9976000000006</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9787.7139000000006</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9827.4305999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10527.8621</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10127.1144</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10098.511</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9673.8487000000005</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9166.0650999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8610.8364999999994</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8690.2245999999996</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8327.8734000000004</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8730.1429000000007</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9137.7896000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8855.9346000000005</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8718.6180999999997</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8885.6825000000008</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8754.5206999999991</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8412.3605000000007</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8739.5948000000008</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>8233.7520999999997</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>8095.8738999999996</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>8192.0923000000003</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>8172.1066000000001</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>7813.1526000000003</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>8040.6850000000004</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>7845.6270999999997</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7920.0464000000002</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>7284.5940000000001</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>7538.5289000000002</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>8268.9195</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>7857.9786999999997</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>7888.6833999999999</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>7741.7843999999996</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>7817.0281000000004</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>8008.4030000000002</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>8200.9938999999995</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>7942.6935000000003</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>8543.1224999999995</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>8716.0208999999995</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>9014.3191999999999</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>8528.2145999999993</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>9012.3588</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>9065.4680000000008</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>8706.8258999999998</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>8763.1874000000007</c:v>
+                </c:pt>
+                <c:pt idx="47" formatCode="General">
+                  <c:v>8886.7255999999998</c:v>
+                </c:pt>
+                <c:pt idx="48" formatCode="General">
+                  <c:v>9378.0524999999998</c:v>
+                </c:pt>
+                <c:pt idx="49" formatCode="General">
+                  <c:v>9341.6980000000003</c:v>
+                </c:pt>
+                <c:pt idx="50" formatCode="General">
+                  <c:v>9014.4318999999996</c:v>
+                </c:pt>
+                <c:pt idx="51" formatCode="General">
+                  <c:v>8814.4061999999994</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-C135-4B1C-A3DE-3E0E7A411B98}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>pivoted!$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>incorrect upper bound</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>pivoted!$B$7:$BA$7</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="52"/>
+                <c:pt idx="1">
+                  <c:v>17209.261299999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15817.402400000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14857.4861</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14192.169400000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13020.537899999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13198.8856</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12921.089</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12831.3513</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13391.534900000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13515.163500000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12722.5754</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12681.3266</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12106.257100000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>11468.2104</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11427.2654</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>11097.3819</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>10797.9175</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>10667.879300000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>10807.639499999999</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>10289.2052</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>10404.6479</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>10376.126099999999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>10128.307699999999</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>10453.893400000001</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>10436.847400000001</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>10071.715</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>10487.572899999999</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>9906.3536000000004</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>10887.806</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>10457.8711</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>9849.4804999999997</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>10035.221299999999</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>10002.116599999999</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>10453.4156</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>9846.9719000000005</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>10169.597</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>10146.206099999999</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>10692.906499999999</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>10476.077499999999</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>10623.579100000001</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>10714.480799999999</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>11035.385399999999</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>10892.0412</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>11203.332</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>11760.774100000001</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>11656.4126</c:v>
+                </c:pt>
+                <c:pt idx="47" formatCode="General">
+                  <c:v>12115.6744</c:v>
+                </c:pt>
+                <c:pt idx="48" formatCode="General">
+                  <c:v>11797.9475</c:v>
+                </c:pt>
+                <c:pt idx="49" formatCode="General">
+                  <c:v>12618.302</c:v>
+                </c:pt>
+                <c:pt idx="50" formatCode="General">
+                  <c:v>13340.3681</c:v>
+                </c:pt>
+                <c:pt idx="51" formatCode="General">
+                  <c:v>14289.193799999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-C135-4B1C-A3DE-3E0E7A411B98}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="595792384"/>
+        <c:axId val="595792056"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="595792384"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="595792056"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="595792056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="22500"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="595792384"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="2500"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -5480,6 +7638,46 @@
 </file>
 
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -7067,6 +9265,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -7174,6 +9888,49 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53B55B01-587E-4818-B7EF-17E0BD10315E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5FDA04AE-34C2-4120-8381-6DF547C87E43}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -21632,7 +24389,7 @@
   <dimension ref="A1:BB25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22239,7 +24996,7 @@
     </row>
     <row r="6" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="7">
@@ -22398,7 +25155,7 @@
     </row>
     <row r="7" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7">
@@ -24933,7 +27690,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C1157C8-6D6A-4CB2-A731-1CE90452F39E}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
@@ -24942,4 +27699,19 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{909EECC5-39A5-4BE0-93C2-7E52FFE2180E}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U4" sqref="U4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add 95% intervals to graph
</commit_message>
<xml_diff>
--- a/data/investigate_sd3.xlsx
+++ b/data/investigate_sd3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\WCA\ons-stats\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{163FB892-7056-4D13-AADD-EF482DD28F6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{928CB565-171B-46E0-ADD3-69FB8B25953B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="1" activeTab="8" xr2:uid="{BACCE0E3-7F96-4AD2-A101-44AECFFFC852}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
   <si>
     <t>DIFF</t>
   </si>
@@ -92,9 +92,6 @@
     <t>Wales</t>
   </si>
   <si>
-    <t>E+W Weekly Deaths (ONS estimate)</t>
-  </si>
-  <si>
     <t>England Weekly Deaths (ONS approx)</t>
   </si>
   <si>
@@ -103,17 +100,27 @@
   <si>
     <t>incorrect upper bound</t>
   </si>
+  <si>
+    <t>Upper 95% confidence interval of estimate</t>
+  </si>
+  <si>
+    <t>Lower 95% confidence interval of estimate</t>
+  </si>
+  <si>
+    <t>Estimated total death occurrences</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="166" formatCode="General_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,13 +141,23 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Helv"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -152,11 +169,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -170,10 +189,21 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
     <cellStyle name="Comma 3" xfId="1" xr:uid="{831DC240-C7B5-4088-91E5-78E571C24AC0}"/>
+    <cellStyle name="Comma 3 13" xfId="2" xr:uid="{29FC539E-6222-4F2B-946E-490731364EA7}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{F8D3DA24-7B56-46CD-A766-B6587D3BB32E}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -295,7 +325,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>pivoted!$A$25</c:f>
+              <c:f>pivoted!$A$28</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -483,7 +513,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>pivoted!$B$25:$BA$25</c:f>
+              <c:f>pivoted!$B$28:$BA$28</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="52"/>
@@ -2008,7 +2038,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>E+W Weekly Deaths (ONS estimate)</c:v>
+                  <c:v>Estimated total death occurrences</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3758,7 +3788,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>E+W Weekly Deaths (ONS estimate)</c:v>
+                  <c:v>Estimated total death occurrences</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5441,7 +5471,21 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>All cause deaths for England and Wales 2020</a:t>
+              <a:t>All cause deaths for England and Wales 2020 by week </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t>of occurrence (ONS data)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>CONTRASTING the effect of different 3SD derivations for upper and lower bounds</a:t>
             </a:r>
           </a:p>
           <a:p>
@@ -5450,7 +5494,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>CONTRASTING the effect of different 3SD derivations</a:t>
+              <a:t>Upper and lower bounds derived from weekly deaths (green) vs daily deaths (red)</a:t>
             </a:r>
           </a:p>
           <a:p>
@@ -5459,17 +5503,9 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>(Upper and lower bounds derived from Weekly Figures)</a:t>
+              <a:t>i.e. mean +/- weekly 3</a:t>
             </a:r>
-          </a:p>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-GB"/>
-              <a:t>i.e. mean +/- weekly 3SD</a:t>
-            </a:r>
+            <a:endParaRPr lang="en-GB"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -5509,15 +5545,387 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="6"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>pivoted!$A$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Upper 95% confidence interval of estimate</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="40000"/>
+                  <a:lumOff val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>pivoted!$B$24:$AV$24</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="47"/>
+                <c:pt idx="0">
+                  <c:v>12505</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12212</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11816</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10979</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11161</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10774</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10942</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10860</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10711</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11050</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10899</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11469</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13870</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>18004</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>22170</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>21047</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>18806</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>15920</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>13794</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>12020</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>11422</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>10284</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>10040</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9525</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>9286</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9744</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>8812</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>8752</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>8982</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>9168</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>8952</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>9090</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>10245</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>8923</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8759</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>9152</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>9234</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>9560</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>9712</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>10104</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>10473</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>10509</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>11227</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>11586</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>11954</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>12871</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>14052</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8A2F-43D3-B786-CE6B25CB6E96}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>pivoted!$A$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Lower 95% confidence interval of estimate</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="40000"/>
+                  <a:lumOff val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>pivoted!$B$25:$AV$25</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="47"/>
+                <c:pt idx="0">
+                  <c:v>12373</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12083</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11691</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10863</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11043</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10660</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10826</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10745</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10597</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10933</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10783</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11348</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13723</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>17814</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>21936</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>20824</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>18607</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>15752</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>13648</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>11893</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>11301</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>10170</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>9924</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9411</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>9167</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9614</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>8693</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>8625</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>8847</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>9027</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>8810</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>8941</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>10076</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>8771</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8605</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>8985</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>9060</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>9374</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>9515</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>9893</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>10247</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>10280</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>10976</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>11318</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>11632</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>12102</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>11343</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-8A2F-43D3-B786-CE6B25CB6E96}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="3"/>
-          <c:order val="0"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
               <c:f>pivoted!$A$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>E+W Weekly Deaths (ONS estimate)</c:v>
+                  <c:v>Estimated total death occurrences</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5858,7 +6266,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="0"/>
-          <c:order val="1"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
               <c:f>pivoted!$A$10</c:f>
@@ -6222,7 +6630,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="2"/>
+          <c:order val="4"/>
           <c:tx>
             <c:strRef>
               <c:f>pivoted!$A$11</c:f>
@@ -6586,7 +6994,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="3"/>
+          <c:order val="5"/>
           <c:tx>
             <c:strRef>
               <c:f>pivoted!$A$12</c:f>
@@ -6950,7 +7358,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
-          <c:order val="4"/>
+          <c:order val="6"/>
           <c:tx>
             <c:strRef>
               <c:f>pivoted!$A$6</c:f>
@@ -7146,7 +7554,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="5"/>
-          <c:order val="5"/>
+          <c:order val="7"/>
           <c:tx>
             <c:strRef>
               <c:f>pivoted!$A$7</c:f>
@@ -7352,7 +7760,7 @@
         <c:axId val="595792384"/>
         <c:axId val="595792056"/>
       </c:lineChart>
-      <c:dateAx>
+      <c:catAx>
         <c:axId val="595792384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
@@ -7413,9 +7821,10 @@
         <c:crossAx val="595792056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:baseTimeUnit val="days"/>
-      </c:dateAx>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
       <c:valAx>
         <c:axId val="595792056"/>
         <c:scaling>
@@ -24386,15 +24795,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6668C7CB-B2D1-4317-91E6-453829098F72}">
-  <dimension ref="A1:BB25"/>
+  <dimension ref="A1:BB29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="54" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -24996,7 +25405,7 @@
     </row>
     <row r="6" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="7">
@@ -25155,7 +25564,7 @@
     </row>
     <row r="7" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7">
@@ -27168,7 +27577,7 @@
     </row>
     <row r="23" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B23" s="7">
         <v>12431</v>
@@ -27314,342 +27723,687 @@
     </row>
     <row r="24" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B24" s="7">
-        <v>756</v>
-      </c>
-      <c r="C24" s="7">
-        <v>856</v>
-      </c>
-      <c r="D24" s="7">
-        <v>812</v>
-      </c>
-      <c r="E24" s="7">
-        <v>802</v>
-      </c>
-      <c r="F24" s="7">
-        <v>760</v>
-      </c>
-      <c r="G24" s="7">
-        <v>729</v>
-      </c>
-      <c r="H24" s="7">
-        <v>722</v>
-      </c>
-      <c r="I24" s="7">
-        <v>724</v>
-      </c>
-      <c r="J24" s="7">
-        <v>698</v>
-      </c>
-      <c r="K24" s="7">
-        <v>720</v>
-      </c>
-      <c r="L24" s="7">
-        <v>727</v>
-      </c>
-      <c r="M24" s="7">
-        <v>677</v>
-      </c>
-      <c r="N24" s="7">
-        <v>665</v>
-      </c>
-      <c r="O24" s="7">
-        <v>667</v>
-      </c>
-      <c r="P24" s="7">
-        <v>671</v>
-      </c>
-      <c r="Q24" s="7">
-        <v>661</v>
-      </c>
-      <c r="R24" s="7">
-        <v>662</v>
-      </c>
-      <c r="S24" s="7">
-        <v>624</v>
-      </c>
-      <c r="T24" s="7">
-        <v>612</v>
-      </c>
-      <c r="U24" s="7">
-        <v>635</v>
-      </c>
-      <c r="V24" s="7">
-        <v>614</v>
-      </c>
-      <c r="W24" s="7">
-        <v>546</v>
-      </c>
-      <c r="X24" s="7">
-        <v>610</v>
-      </c>
-      <c r="Y24" s="7">
-        <v>588</v>
-      </c>
-      <c r="Z24" s="7">
-        <v>573</v>
-      </c>
-      <c r="AA24" s="7">
-        <v>571</v>
-      </c>
-      <c r="AB24" s="7">
-        <v>555</v>
-      </c>
-      <c r="AC24" s="7">
-        <v>578</v>
-      </c>
-      <c r="AD24" s="7">
-        <v>557</v>
-      </c>
-      <c r="AE24" s="7">
-        <v>566</v>
-      </c>
-      <c r="AF24" s="7">
-        <v>572</v>
-      </c>
-      <c r="AG24" s="7">
-        <v>571</v>
-      </c>
-      <c r="AH24" s="7">
-        <v>564</v>
-      </c>
-      <c r="AI24" s="7">
-        <v>573</v>
-      </c>
-      <c r="AJ24" s="7">
-        <v>539</v>
-      </c>
-      <c r="AK24" s="7">
-        <v>552</v>
-      </c>
-      <c r="AL24" s="7">
-        <v>577</v>
-      </c>
-      <c r="AM24" s="7">
-        <v>575</v>
-      </c>
-      <c r="AN24" s="7">
-        <v>604</v>
-      </c>
-      <c r="AO24" s="7">
-        <v>587</v>
-      </c>
-      <c r="AP24" s="7">
-        <v>615</v>
-      </c>
-      <c r="AQ24" s="7">
-        <v>630</v>
-      </c>
-      <c r="AR24" s="7">
-        <v>628</v>
-      </c>
-      <c r="AS24" s="7">
-        <v>616</v>
-      </c>
-      <c r="AT24" s="7">
-        <v>625</v>
-      </c>
-      <c r="AU24" s="7">
-        <v>658</v>
-      </c>
-      <c r="AV24" s="7">
-        <v>653</v>
+        <v>22</v>
+      </c>
+      <c r="B24" s="9">
+        <v>12505</v>
+      </c>
+      <c r="C24" s="9">
+        <v>12212</v>
+      </c>
+      <c r="D24" s="9">
+        <v>11816</v>
+      </c>
+      <c r="E24" s="9">
+        <v>10979</v>
+      </c>
+      <c r="F24" s="9">
+        <v>11161</v>
+      </c>
+      <c r="G24" s="9">
+        <v>10774</v>
+      </c>
+      <c r="H24" s="9">
+        <v>10942</v>
+      </c>
+      <c r="I24" s="9">
+        <v>10860</v>
+      </c>
+      <c r="J24" s="9">
+        <v>10711</v>
+      </c>
+      <c r="K24" s="9">
+        <v>11050</v>
+      </c>
+      <c r="L24" s="9">
+        <v>10899</v>
+      </c>
+      <c r="M24" s="9">
+        <v>11469</v>
+      </c>
+      <c r="N24" s="9">
+        <v>13870</v>
+      </c>
+      <c r="O24" s="9">
+        <v>18004</v>
+      </c>
+      <c r="P24" s="9">
+        <v>22170</v>
+      </c>
+      <c r="Q24" s="9">
+        <v>21047</v>
+      </c>
+      <c r="R24" s="9">
+        <v>18806</v>
+      </c>
+      <c r="S24" s="9">
+        <v>15920</v>
+      </c>
+      <c r="T24" s="9">
+        <v>13794</v>
+      </c>
+      <c r="U24" s="9">
+        <v>12020</v>
+      </c>
+      <c r="V24" s="9">
+        <v>11422</v>
+      </c>
+      <c r="W24" s="9">
+        <v>10284</v>
+      </c>
+      <c r="X24" s="9">
+        <v>10040</v>
+      </c>
+      <c r="Y24" s="9">
+        <v>9525</v>
+      </c>
+      <c r="Z24" s="9">
+        <v>9286</v>
+      </c>
+      <c r="AA24" s="9">
+        <v>9744</v>
+      </c>
+      <c r="AB24" s="9">
+        <v>8812</v>
+      </c>
+      <c r="AC24" s="9">
+        <v>8752</v>
+      </c>
+      <c r="AD24" s="9">
+        <v>8982</v>
+      </c>
+      <c r="AE24" s="9">
+        <v>9168</v>
+      </c>
+      <c r="AF24" s="9">
+        <v>8952</v>
+      </c>
+      <c r="AG24" s="9">
+        <v>9090</v>
+      </c>
+      <c r="AH24" s="9">
+        <v>10245</v>
+      </c>
+      <c r="AI24" s="9">
+        <v>8923</v>
+      </c>
+      <c r="AJ24" s="9">
+        <v>8759</v>
+      </c>
+      <c r="AK24" s="9">
+        <v>9152</v>
+      </c>
+      <c r="AL24" s="9">
+        <v>9234</v>
+      </c>
+      <c r="AM24" s="9">
+        <v>9560</v>
+      </c>
+      <c r="AN24" s="9">
+        <v>9712</v>
+      </c>
+      <c r="AO24" s="9">
+        <v>10104</v>
+      </c>
+      <c r="AP24" s="9">
+        <v>10473</v>
+      </c>
+      <c r="AQ24" s="9">
+        <v>10509</v>
+      </c>
+      <c r="AR24" s="9">
+        <v>11227</v>
+      </c>
+      <c r="AS24" s="9">
+        <v>11586</v>
+      </c>
+      <c r="AT24" s="10">
+        <v>11954</v>
+      </c>
+      <c r="AU24" s="10">
+        <v>12871</v>
+      </c>
+      <c r="AV24" s="11">
+        <v>14052</v>
       </c>
     </row>
     <row r="25" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B25" s="7">
-        <f>B23-B24</f>
+        <v>23</v>
+      </c>
+      <c r="B25" s="9">
+        <v>12373</v>
+      </c>
+      <c r="C25" s="9">
+        <v>12083</v>
+      </c>
+      <c r="D25" s="9">
+        <v>11691</v>
+      </c>
+      <c r="E25" s="9">
+        <v>10863</v>
+      </c>
+      <c r="F25" s="9">
+        <v>11043</v>
+      </c>
+      <c r="G25" s="9">
+        <v>10660</v>
+      </c>
+      <c r="H25" s="9">
+        <v>10826</v>
+      </c>
+      <c r="I25" s="9">
+        <v>10745</v>
+      </c>
+      <c r="J25" s="9">
+        <v>10597</v>
+      </c>
+      <c r="K25" s="9">
+        <v>10933</v>
+      </c>
+      <c r="L25" s="9">
+        <v>10783</v>
+      </c>
+      <c r="M25" s="9">
+        <v>11348</v>
+      </c>
+      <c r="N25" s="9">
+        <v>13723</v>
+      </c>
+      <c r="O25" s="9">
+        <v>17814</v>
+      </c>
+      <c r="P25" s="9">
+        <v>21936</v>
+      </c>
+      <c r="Q25" s="9">
+        <v>20824</v>
+      </c>
+      <c r="R25" s="9">
+        <v>18607</v>
+      </c>
+      <c r="S25" s="9">
+        <v>15752</v>
+      </c>
+      <c r="T25" s="9">
+        <v>13648</v>
+      </c>
+      <c r="U25" s="9">
+        <v>11893</v>
+      </c>
+      <c r="V25" s="9">
+        <v>11301</v>
+      </c>
+      <c r="W25" s="9">
+        <v>10170</v>
+      </c>
+      <c r="X25" s="9">
+        <v>9924</v>
+      </c>
+      <c r="Y25" s="9">
+        <v>9411</v>
+      </c>
+      <c r="Z25" s="9">
+        <v>9167</v>
+      </c>
+      <c r="AA25" s="9">
+        <v>9614</v>
+      </c>
+      <c r="AB25" s="9">
+        <v>8693</v>
+      </c>
+      <c r="AC25" s="9">
+        <v>8625</v>
+      </c>
+      <c r="AD25" s="9">
+        <v>8847</v>
+      </c>
+      <c r="AE25" s="9">
+        <v>9027</v>
+      </c>
+      <c r="AF25" s="9">
+        <v>8810</v>
+      </c>
+      <c r="AG25" s="9">
+        <v>8941</v>
+      </c>
+      <c r="AH25" s="9">
+        <v>10076</v>
+      </c>
+      <c r="AI25" s="9">
+        <v>8771</v>
+      </c>
+      <c r="AJ25" s="9">
+        <v>8605</v>
+      </c>
+      <c r="AK25" s="9">
+        <v>8985</v>
+      </c>
+      <c r="AL25" s="9">
+        <v>9060</v>
+      </c>
+      <c r="AM25" s="9">
+        <v>9374</v>
+      </c>
+      <c r="AN25" s="9">
+        <v>9515</v>
+      </c>
+      <c r="AO25" s="9">
+        <v>9893</v>
+      </c>
+      <c r="AP25" s="9">
+        <v>10247</v>
+      </c>
+      <c r="AQ25" s="9">
+        <v>10280</v>
+      </c>
+      <c r="AR25" s="9">
+        <v>10976</v>
+      </c>
+      <c r="AS25" s="9">
+        <v>11318</v>
+      </c>
+      <c r="AT25" s="10">
+        <v>11632</v>
+      </c>
+      <c r="AU25" s="10">
+        <v>12102</v>
+      </c>
+      <c r="AV25" s="11">
+        <v>11343</v>
+      </c>
+    </row>
+    <row r="26" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A26" s="4"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
+      <c r="N26" s="7"/>
+      <c r="O26" s="7"/>
+      <c r="P26" s="7"/>
+      <c r="Q26" s="7"/>
+      <c r="R26" s="7"/>
+      <c r="S26" s="7"/>
+      <c r="T26" s="7"/>
+      <c r="U26" s="7"/>
+      <c r="V26" s="7"/>
+      <c r="W26" s="7"/>
+      <c r="X26" s="7"/>
+      <c r="Y26" s="7"/>
+      <c r="Z26" s="7"/>
+      <c r="AA26" s="7"/>
+      <c r="AB26" s="7"/>
+      <c r="AC26" s="7"/>
+      <c r="AD26" s="7"/>
+      <c r="AE26" s="7"/>
+      <c r="AF26" s="7"/>
+      <c r="AG26" s="7"/>
+      <c r="AH26" s="7"/>
+      <c r="AI26" s="7"/>
+      <c r="AJ26" s="7"/>
+      <c r="AK26" s="7"/>
+      <c r="AL26" s="7"/>
+      <c r="AM26" s="7"/>
+      <c r="AN26" s="7"/>
+      <c r="AO26" s="7"/>
+      <c r="AP26" s="7"/>
+      <c r="AQ26" s="7"/>
+      <c r="AR26" s="7"/>
+      <c r="AS26" s="7"/>
+      <c r="AT26" s="7"/>
+      <c r="AU26" s="7"/>
+      <c r="AV26" s="7"/>
+    </row>
+    <row r="27" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B27" s="7">
+        <v>756</v>
+      </c>
+      <c r="C27" s="7">
+        <v>856</v>
+      </c>
+      <c r="D27" s="7">
+        <v>812</v>
+      </c>
+      <c r="E27" s="7">
+        <v>802</v>
+      </c>
+      <c r="F27" s="7">
+        <v>760</v>
+      </c>
+      <c r="G27" s="7">
+        <v>729</v>
+      </c>
+      <c r="H27" s="7">
+        <v>722</v>
+      </c>
+      <c r="I27" s="7">
+        <v>724</v>
+      </c>
+      <c r="J27" s="7">
+        <v>698</v>
+      </c>
+      <c r="K27" s="7">
+        <v>720</v>
+      </c>
+      <c r="L27" s="7">
+        <v>727</v>
+      </c>
+      <c r="M27" s="7">
+        <v>677</v>
+      </c>
+      <c r="N27" s="7">
+        <v>665</v>
+      </c>
+      <c r="O27" s="7">
+        <v>667</v>
+      </c>
+      <c r="P27" s="7">
+        <v>671</v>
+      </c>
+      <c r="Q27" s="7">
+        <v>661</v>
+      </c>
+      <c r="R27" s="7">
+        <v>662</v>
+      </c>
+      <c r="S27" s="7">
+        <v>624</v>
+      </c>
+      <c r="T27" s="7">
+        <v>612</v>
+      </c>
+      <c r="U27" s="7">
+        <v>635</v>
+      </c>
+      <c r="V27" s="7">
+        <v>614</v>
+      </c>
+      <c r="W27" s="7">
+        <v>546</v>
+      </c>
+      <c r="X27" s="7">
+        <v>610</v>
+      </c>
+      <c r="Y27" s="7">
+        <v>588</v>
+      </c>
+      <c r="Z27" s="7">
+        <v>573</v>
+      </c>
+      <c r="AA27" s="7">
+        <v>571</v>
+      </c>
+      <c r="AB27" s="7">
+        <v>555</v>
+      </c>
+      <c r="AC27" s="7">
+        <v>578</v>
+      </c>
+      <c r="AD27" s="7">
+        <v>557</v>
+      </c>
+      <c r="AE27" s="7">
+        <v>566</v>
+      </c>
+      <c r="AF27" s="7">
+        <v>572</v>
+      </c>
+      <c r="AG27" s="7">
+        <v>571</v>
+      </c>
+      <c r="AH27" s="7">
+        <v>564</v>
+      </c>
+      <c r="AI27" s="7">
+        <v>573</v>
+      </c>
+      <c r="AJ27" s="7">
+        <v>539</v>
+      </c>
+      <c r="AK27" s="7">
+        <v>552</v>
+      </c>
+      <c r="AL27" s="7">
+        <v>577</v>
+      </c>
+      <c r="AM27" s="7">
+        <v>575</v>
+      </c>
+      <c r="AN27" s="7">
+        <v>604</v>
+      </c>
+      <c r="AO27" s="7">
+        <v>587</v>
+      </c>
+      <c r="AP27" s="7">
+        <v>615</v>
+      </c>
+      <c r="AQ27" s="7">
+        <v>630</v>
+      </c>
+      <c r="AR27" s="7">
+        <v>628</v>
+      </c>
+      <c r="AS27" s="7">
+        <v>616</v>
+      </c>
+      <c r="AT27" s="7">
+        <v>625</v>
+      </c>
+      <c r="AU27" s="7">
+        <v>658</v>
+      </c>
+      <c r="AV27" s="7">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="28" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28" s="7">
+        <f>B23-B27</f>
         <v>11675</v>
       </c>
-      <c r="C25" s="7">
-        <f t="shared" ref="C25:AV25" si="3">C23-C24</f>
+      <c r="C28" s="7">
+        <f t="shared" ref="C28:AV28" si="3">C23-C27</f>
         <v>11283</v>
       </c>
-      <c r="D25" s="7">
+      <c r="D28" s="7">
         <f t="shared" si="3"/>
         <v>10934</v>
       </c>
-      <c r="E25" s="7">
+      <c r="E28" s="7">
         <f t="shared" si="3"/>
         <v>10112</v>
       </c>
-      <c r="F25" s="7">
+      <c r="F28" s="7">
         <f t="shared" si="3"/>
         <v>10334</v>
       </c>
-      <c r="G25" s="7">
+      <c r="G28" s="7">
         <f t="shared" si="3"/>
         <v>9981</v>
       </c>
-      <c r="H25" s="7">
+      <c r="H28" s="7">
         <f t="shared" si="3"/>
         <v>10155</v>
       </c>
-      <c r="I25" s="7">
+      <c r="I28" s="7">
         <f t="shared" si="3"/>
         <v>10071</v>
       </c>
-      <c r="J25" s="7">
+      <c r="J28" s="7">
         <f t="shared" si="3"/>
         <v>9949</v>
       </c>
-      <c r="K25" s="7">
+      <c r="K28" s="7">
         <f t="shared" si="3"/>
         <v>10264</v>
       </c>
-      <c r="L25" s="7">
+      <c r="L28" s="7">
         <f t="shared" si="3"/>
         <v>10107</v>
       </c>
-      <c r="M25" s="7">
+      <c r="M28" s="7">
         <f t="shared" si="3"/>
         <v>10724</v>
       </c>
-      <c r="N25" s="7">
+      <c r="N28" s="7">
         <f t="shared" si="3"/>
         <v>13122</v>
       </c>
-      <c r="O25" s="7">
+      <c r="O28" s="7">
         <f t="shared" si="3"/>
         <v>17230</v>
       </c>
-      <c r="P25" s="7">
+      <c r="P28" s="7">
         <f t="shared" si="3"/>
         <v>21367</v>
       </c>
-      <c r="Q25" s="7">
+      <c r="Q28" s="7">
         <f t="shared" si="3"/>
         <v>20261</v>
       </c>
-      <c r="R25" s="7">
+      <c r="R28" s="7">
         <f t="shared" si="3"/>
         <v>18032</v>
       </c>
-      <c r="S25" s="7">
+      <c r="S28" s="7">
         <f t="shared" si="3"/>
         <v>15201</v>
       </c>
-      <c r="T25" s="7">
+      <c r="T28" s="7">
         <f t="shared" si="3"/>
         <v>13100</v>
       </c>
-      <c r="U25" s="7">
+      <c r="U28" s="7">
         <f t="shared" si="3"/>
         <v>11313</v>
       </c>
-      <c r="V25" s="7">
+      <c r="V28" s="7">
         <f t="shared" si="3"/>
         <v>10740</v>
       </c>
-      <c r="W25" s="7">
+      <c r="W28" s="7">
         <f t="shared" si="3"/>
         <v>9674</v>
       </c>
-      <c r="X25" s="7">
+      <c r="X28" s="7">
         <f t="shared" si="3"/>
         <v>9365</v>
       </c>
-      <c r="Y25" s="7">
+      <c r="Y28" s="7">
         <f t="shared" si="3"/>
         <v>8874</v>
       </c>
-      <c r="Z25" s="7">
+      <c r="Z28" s="7">
         <f t="shared" si="3"/>
         <v>8647</v>
       </c>
-      <c r="AA25" s="7">
+      <c r="AA28" s="7">
         <f t="shared" si="3"/>
         <v>9100</v>
       </c>
-      <c r="AB25" s="7">
+      <c r="AB28" s="7">
         <f t="shared" si="3"/>
         <v>8191</v>
       </c>
-      <c r="AC25" s="7">
+      <c r="AC28" s="7">
         <f t="shared" si="3"/>
         <v>8104</v>
       </c>
-      <c r="AD25" s="7">
+      <c r="AD28" s="7">
         <f t="shared" si="3"/>
         <v>8350</v>
       </c>
-      <c r="AE25" s="7">
+      <c r="AE28" s="7">
         <f t="shared" si="3"/>
         <v>8524</v>
       </c>
-      <c r="AF25" s="7">
+      <c r="AF28" s="7">
         <f t="shared" si="3"/>
         <v>8302</v>
       </c>
-      <c r="AG25" s="7">
+      <c r="AG28" s="7">
         <f t="shared" si="3"/>
         <v>8438</v>
       </c>
-      <c r="AH25" s="7">
+      <c r="AH28" s="7">
         <f t="shared" si="3"/>
         <v>9589</v>
       </c>
-      <c r="AI25" s="7">
+      <c r="AI28" s="7">
         <f t="shared" si="3"/>
         <v>8267</v>
       </c>
-      <c r="AJ25" s="7">
+      <c r="AJ28" s="7">
         <f t="shared" si="3"/>
         <v>8136</v>
       </c>
-      <c r="AK25" s="7">
+      <c r="AK28" s="7">
         <f t="shared" si="3"/>
         <v>8509</v>
       </c>
-      <c r="AL25" s="7">
+      <c r="AL28" s="7">
         <f t="shared" si="3"/>
         <v>8563</v>
       </c>
-      <c r="AM25" s="7">
+      <c r="AM28" s="7">
         <f t="shared" si="3"/>
         <v>8885</v>
       </c>
-      <c r="AN25" s="7">
+      <c r="AN28" s="7">
         <f t="shared" si="3"/>
         <v>9001</v>
       </c>
-      <c r="AO25" s="7">
+      <c r="AO28" s="7">
         <f t="shared" si="3"/>
         <v>9403</v>
       </c>
-      <c r="AP25" s="7">
+      <c r="AP28" s="7">
         <f t="shared" si="3"/>
         <v>9736</v>
       </c>
-      <c r="AQ25" s="7">
+      <c r="AQ28" s="7">
         <f t="shared" si="3"/>
         <v>9756</v>
       </c>
-      <c r="AR25" s="7">
+      <c r="AR28" s="7">
         <f t="shared" si="3"/>
         <v>10464</v>
       </c>
-      <c r="AS25" s="7">
+      <c r="AS28" s="7">
         <f t="shared" si="3"/>
         <v>10826</v>
       </c>
-      <c r="AT25" s="7">
+      <c r="AT28" s="7">
         <f t="shared" si="3"/>
         <v>11156</v>
       </c>
-      <c r="AU25" s="7">
+      <c r="AU28" s="7">
         <f t="shared" si="3"/>
         <v>11788</v>
       </c>
-      <c r="AV25" s="7">
+      <c r="AV28" s="7">
         <f t="shared" si="3"/>
         <v>11913</v>
       </c>
+    </row>
+    <row r="29" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -27706,7 +28460,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U4" sqref="U4"/>
+      <selection activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Use darker red for COVID deaths
</commit_message>
<xml_diff>
--- a/data/investigate_sd3.xlsx
+++ b/data/investigate_sd3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\WCA\ons-stats\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72E008E3-3675-4689-B0D3-7022E754A3B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6B4BABC-B1F5-4A19-BDE1-15065BD3E41F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="1" activeTab="8" xr2:uid="{BACCE0E3-7F96-4AD2-A101-44AECFFFC852}"/>
   </bookViews>
@@ -6294,7 +6294,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="FF0000"/>
+                <a:srgbClr val="C00000"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -28803,7 +28803,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V3" sqref="V3"/>
+      <selection activeCell="V15" sqref="V15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add non-COVID deaths in green
</commit_message>
<xml_diff>
--- a/data/investigate_sd3.xlsx
+++ b/data/investigate_sd3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\WCA\ons-stats\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6B4BABC-B1F5-4A19-BDE1-15065BD3E41F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C8D0FD3-A066-47C1-A824-E32037AA1D0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="1" activeTab="8" xr2:uid="{BACCE0E3-7F96-4AD2-A101-44AECFFFC852}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="699" firstSheet="2" activeTab="9" xr2:uid="{BACCE0E3-7F96-4AD2-A101-44AECFFFC852}"/>
   </bookViews>
   <sheets>
     <sheet name="daily_phe" sheetId="6" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="daily_limits" sheetId="4" r:id="rId7"/>
     <sheet name="weekly_limits" sheetId="5" r:id="rId8"/>
     <sheet name="sd3_comparison" sheetId="9" r:id="rId9"/>
+    <sheet name="other_causes" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
   <si>
     <t>DIFF</t>
   </si>
@@ -111,6 +112,9 @@
   </si>
   <si>
     <t>Deaths involving COVID-19, all ages</t>
+  </si>
+  <si>
+    <t>Deaths from other causes</t>
   </si>
 </sst>
 </file>
@@ -8162,6 +8166,2901 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>All cause deaths for England and Wales 2020 by week </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t>of occurrence (ONS data)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>CONTRASTING the effect of different 3SD derivations for upper and lower bounds</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Upper and lower bounds derived from weekly deaths (green) vs daily deaths (red)</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>i.e. mean +/- weekly 3</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>pivoted!$A$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Upper 95% confidence interval of estimate</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="40000"/>
+                  <a:lumOff val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>pivoted!$B$24:$AV$24</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="47"/>
+                <c:pt idx="0">
+                  <c:v>12505</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12212</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11816</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10979</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11161</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10774</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10942</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10860</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10711</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11050</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10899</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11469</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13870</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>18004</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>22170</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>21047</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>18806</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>15920</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>13794</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>12020</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>11422</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>10284</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>10040</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9525</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>9286</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9744</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>8812</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>8752</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>8982</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>9168</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>8952</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>9090</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>10245</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>8923</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8759</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>9152</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>9234</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>9560</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>9712</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>10104</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>10473</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>10509</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>11227</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>11586</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>11954</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>12871</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>14052</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6A80-46A0-99E3-3B20F67D5A48}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>pivoted!$A$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Lower 95% confidence interval of estimate</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="40000"/>
+                  <a:lumOff val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>pivoted!$B$25:$AV$25</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="47"/>
+                <c:pt idx="0">
+                  <c:v>12373</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12083</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11691</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10863</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11043</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10660</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10826</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10745</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10597</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10933</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10783</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11348</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13723</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>17814</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>21936</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>20824</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>18607</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>15752</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>13648</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>11893</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>11301</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>10170</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>9924</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9411</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>9167</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9614</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>8693</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>8625</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>8847</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>9027</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>8810</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>8941</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>10076</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>8771</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8605</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>8985</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>9060</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>9374</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>9515</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>9893</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>10247</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>10280</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>10976</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>11318</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>11632</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>12102</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>11343</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6A80-46A0-99E3-3B20F67D5A48}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>pivoted!$A$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Estimated total death occurrences</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>pivoted!$B$2:$BA$2</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="52"/>
+                <c:pt idx="0">
+                  <c:v>43833</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43840</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43847</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43854</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43861</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43868</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43875</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43882</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43889</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43896</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43903</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>43910</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43917</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>43924</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>43931</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>43938</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>43945</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>43952</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>43959</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>43966</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>43973</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>43980</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43987</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>43994</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>44001</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>44008</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>44015</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>44022</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>44029</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>44036</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>44043</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>44050</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>44057</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>44064</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>44071</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>44078</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>44085</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>44092</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>44099</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>44106</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>44113</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>44120</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>44127</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44134</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>44141</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>44148</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>44155</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>44162</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>44169</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>44176</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>44183</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>44190</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>pivoted!$B$23:$BB$23</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="53"/>
+                <c:pt idx="0">
+                  <c:v>12431</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12139</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11746</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10914</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11094</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10710</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10877</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10795</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10647</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10984</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10834</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11401</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13787</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>17897</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>22038</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>20922</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>18694</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>15825</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>13712</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>11948</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>11354</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>10220</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>9975</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9462</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>9220</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9671</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>8746</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>8682</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>8907</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>9090</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>8874</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>9009</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>10153</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>8840</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8675</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>9061</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>9140</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>9460</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>9605</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>9990</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>10351</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>10386</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>11092</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>11442</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>11781</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>12446</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>12566</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-6A80-46A0-99E3-3B20F67D5A48}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>pivoted!$A$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Deaths involving COVID-19, all ages</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>pivoted!$B$30:$AV$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="47"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>404</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1882</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5190</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8252</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8322</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6946</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5219</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3989</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2862</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2284</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1781</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1310</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>950</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>678</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>588</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>425</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>336</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>233</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>193</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>163</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>133</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>168</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>244</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>378</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>526</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>768</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1263</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1665</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2179</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2563</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2549</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-6A80-46A0-99E3-3B20F67D5A48}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>pivoted!$A$31</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Deaths from other causes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>pivoted!$B$31:$AV$31</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="47"/>
+                <c:pt idx="0">
+                  <c:v>12431</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12139</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11746</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10914</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11093</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10709</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10877</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10795</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10646</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10978</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10790</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10997</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11905</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12707</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>13786</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>12600</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>11748</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>10606</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9723</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9086</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9070</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>8439</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>8665</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>8512</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>8542</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9083</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>8321</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>8346</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>8674</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>8897</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>8711</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>8876</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>10013</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>8739</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8583</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>8984</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>9040</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>9292</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>9361</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>9612</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>9825</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>9618</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>9829</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>9777</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>9602</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>9883</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>10017</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-6A80-46A0-99E3-3B20F67D5A48}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>pivoted!$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>baseline</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>pivoted!$B$2:$BA$2</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="52"/>
+                <c:pt idx="0">
+                  <c:v>43833</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43840</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43847</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43854</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43861</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43868</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43875</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43882</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43889</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43896</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43903</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>43910</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43917</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>43924</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>43931</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>43938</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>43945</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>43952</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>43959</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>43966</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>43973</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>43980</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43987</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>43994</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>44001</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>44008</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>44015</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>44022</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>44029</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>44036</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>44043</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>44050</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>44057</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>44064</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>44071</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>44078</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>44085</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>44092</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>44099</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>44106</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>44113</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>44120</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>44127</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44134</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>44141</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>44148</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>44155</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>44162</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>44169</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>44176</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>44183</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>44190</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>pivoted!$B$10:$BB$10</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="53"/>
+                <c:pt idx="0">
+                  <c:v>12700.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12895</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12618.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12173.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12079.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11670.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11660.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11402.4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11323.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11252.8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10910</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10607.2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10448.799999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10360.4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>10263.4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10084.799999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9812.2000000000007</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9743.7999999999993</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9746</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9537</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9500.2000000000007</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9197</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>9223.4</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9205.6</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>9275</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9051.6</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>9271.6</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>8903</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>9113.4</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>9125.7999999999993</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>8783.6</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>9050</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>9013.7999999999993</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>8974.7999999999993</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8939.2000000000007</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>8922.2000000000007</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>9132.6</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>9204</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>9450.4</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>9530.2000000000007</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>9812</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>9843.7999999999993</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>9823</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>10082.200000000001</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>10192.200000000001</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>10227.200000000001</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>10296.4</c:v>
+                </c:pt>
+                <c:pt idx="47" formatCode="General">
+                  <c:v>10467.6</c:v>
+                </c:pt>
+                <c:pt idx="48" formatCode="General">
+                  <c:v>10857.2</c:v>
+                </c:pt>
+                <c:pt idx="49" formatCode="General">
+                  <c:v>11032</c:v>
+                </c:pt>
+                <c:pt idx="50" formatCode="General">
+                  <c:v>11396.8</c:v>
+                </c:pt>
+                <c:pt idx="51" formatCode="General">
+                  <c:v>11616</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-6A80-46A0-99E3-3B20F67D5A48}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>pivoted!$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>lower bound</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>pivoted!$B$2:$BA$2</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="52"/>
+                <c:pt idx="0">
+                  <c:v>43833</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43840</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43847</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43854</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43861</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43868</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43875</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43882</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43889</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43896</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43903</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>43910</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43917</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>43924</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>43931</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>43938</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>43945</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>43952</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>43959</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>43966</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>43973</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>43980</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43987</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>43994</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>44001</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>44008</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>44015</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>44022</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>44029</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>44036</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>44043</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>44050</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>44057</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>44064</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>44071</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>44078</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>44085</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>44092</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>44099</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>44106</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>44113</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>44120</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>44127</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44134</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>44141</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>44148</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>44155</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>44162</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>44169</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>44176</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>44183</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>44190</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>pivoted!$B$11:$BB$11</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="53"/>
+                <c:pt idx="0">
+                  <c:v>8538.0867999999991</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8859.8883000000005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9487.9120000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9766.1206000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10183.6754</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10741.7268</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10312.0226</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10287.0476</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9681.7263000000003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8645.9298999999992</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8646.4256999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8834.4945000000007</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8910.5640000000003</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9045.2188999999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9289.3917000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9012.3541000000005</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9069.3176000000003</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9446.6067000000003</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9135.9707999999991</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9131.6023999999998</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8612.6898999999994</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>8823.0262000000002</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>8387.6566000000003</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>8865.0313999999998</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>8146.2088000000003</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8409.7553000000007</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>8917.8055000000004</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>8380.7034999999996</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7724.7446</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>7841.0384999999997</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>8437.9010999999991</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>8786.0545999999995</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>8084.2677000000003</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>8504.6916999999994</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8182.7420000000002</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>8445.2682999999997</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>8829.2491000000009</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>8335.9698000000008</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>8700.8906999999999</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>9071.5064000000002</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>9390.7932000000001</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>8966.1036000000004</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>9066.3883000000005</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>9625.5949000000001</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>9386.9307000000008</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>9003.7245000000003</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>8748.8808000000008</c:v>
+                </c:pt>
+                <c:pt idx="47" formatCode="General">
+                  <c:v>9592.7255000000005</c:v>
+                </c:pt>
+                <c:pt idx="48" formatCode="General">
+                  <c:v>9675.4673999999995</c:v>
+                </c:pt>
+                <c:pt idx="49" formatCode="General">
+                  <c:v>9200.7934999999998</c:v>
+                </c:pt>
+                <c:pt idx="50" formatCode="General">
+                  <c:v>8975.6031000000003</c:v>
+                </c:pt>
+                <c:pt idx="51" formatCode="General">
+                  <c:v>8860.8042000000005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-6A80-46A0-99E3-3B20F67D5A48}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>pivoted!$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>upper bound</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>pivoted!$B$2:$BA$2</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="52"/>
+                <c:pt idx="0">
+                  <c:v>43833</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43840</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43847</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43854</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43861</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43868</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43875</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43882</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43889</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43896</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43903</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>43910</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43917</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>43924</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>43931</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>43938</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>43945</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>43952</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>43959</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>43966</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>43973</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>43980</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43987</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>43994</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>44001</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>44008</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>44015</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>44022</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>44029</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>44036</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>44043</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>44050</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>44057</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>44064</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>44071</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>44078</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>44085</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>44092</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>44099</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>44106</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>44113</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>44120</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>44127</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44134</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>44141</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>44148</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>44155</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>44162</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>44169</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>44176</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>44183</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>44190</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>pivoted!$B$12:$BB$12</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="53"/>
+                <c:pt idx="0">
+                  <c:v>16862.713199999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16930.111700000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15749.288</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14580.679400000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13975.524600000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12599.8732</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13009.1774</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12517.752399999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12964.673699999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13859.670099999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13173.5743</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12379.905500000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11987.036</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>11675.581099999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>11237.408299999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11157.2459</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>10555.082399999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>10040.9933</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>10356.029200000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9942.3976000000002</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>10387.7101</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9570.9737999999998</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>10059.143400000001</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9546.1686000000009</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>10403.7912</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9693.4447</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>9625.3945000000003</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>9425.2965000000004</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>10502.055399999999</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>10410.5615</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>9129.2988999999998</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>9313.9454000000005</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>9943.3323</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>9444.9082999999991</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>9695.6579999999994</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>9399.1316999999999</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>9435.9508999999998</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>10072.030199999999</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>10199.909299999999</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>9988.8935999999994</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>10233.2068</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>10721.4964</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>10579.611699999999</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>10538.8051</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>10997.469300000001</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>11450.675499999999</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>11843.9192</c:v>
+                </c:pt>
+                <c:pt idx="47" formatCode="General">
+                  <c:v>11342.4745</c:v>
+                </c:pt>
+                <c:pt idx="48" formatCode="General">
+                  <c:v>12038.9326</c:v>
+                </c:pt>
+                <c:pt idx="49" formatCode="General">
+                  <c:v>12863.2065</c:v>
+                </c:pt>
+                <c:pt idx="50" formatCode="General">
+                  <c:v>13817.9969</c:v>
+                </c:pt>
+                <c:pt idx="51" formatCode="General">
+                  <c:v>14371.1958</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-6A80-46A0-99E3-3B20F67D5A48}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>pivoted!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>incorrect lower bound</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>pivoted!$B$6:$BA$6</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="52"/>
+                <c:pt idx="1">
+                  <c:v>8691.5386999999992</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9298.9976000000006</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9787.7139000000006</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9827.4305999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10527.8621</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10127.1144</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10098.511</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9673.8487000000005</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9166.0650999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8610.8364999999994</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8690.2245999999996</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8327.8734000000004</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8730.1429000000007</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9137.7896000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8855.9346000000005</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8718.6180999999997</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8885.6825000000008</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8754.5206999999991</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8412.3605000000007</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8739.5948000000008</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>8233.7520999999997</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>8095.8738999999996</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>8192.0923000000003</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>8172.1066000000001</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>7813.1526000000003</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>8040.6850000000004</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>7845.6270999999997</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7920.0464000000002</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>7284.5940000000001</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>7538.5289000000002</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>8268.9195</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>7857.9786999999997</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>7888.6833999999999</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>7741.7843999999996</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>7817.0281000000004</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>8008.4030000000002</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>8200.9938999999995</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>7942.6935000000003</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>8543.1224999999995</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>8716.0208999999995</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>9014.3191999999999</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>8528.2145999999993</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>9012.3588</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>9065.4680000000008</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>8706.8258999999998</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>8763.1874000000007</c:v>
+                </c:pt>
+                <c:pt idx="47" formatCode="General">
+                  <c:v>8886.7255999999998</c:v>
+                </c:pt>
+                <c:pt idx="48" formatCode="General">
+                  <c:v>9378.0524999999998</c:v>
+                </c:pt>
+                <c:pt idx="49" formatCode="General">
+                  <c:v>9341.6980000000003</c:v>
+                </c:pt>
+                <c:pt idx="50" formatCode="General">
+                  <c:v>9014.4318999999996</c:v>
+                </c:pt>
+                <c:pt idx="51" formatCode="General">
+                  <c:v>8814.4061999999994</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-6A80-46A0-99E3-3B20F67D5A48}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>pivoted!$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>incorrect upper bound</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>pivoted!$B$7:$BA$7</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="52"/>
+                <c:pt idx="1">
+                  <c:v>17209.261299999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15817.402400000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14857.4861</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14192.169400000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13020.537899999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13198.8856</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12921.089</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12831.3513</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13391.534900000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13515.163500000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12722.5754</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12681.3266</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12106.257100000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>11468.2104</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11427.2654</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>11097.3819</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>10797.9175</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>10667.879300000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>10807.639499999999</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>10289.2052</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>10404.6479</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>10376.126099999999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>10128.307699999999</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>10453.893400000001</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>10436.847400000001</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>10071.715</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>10487.572899999999</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>9906.3536000000004</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>10887.806</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>10457.8711</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>9849.4804999999997</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>10035.221299999999</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>10002.116599999999</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>10453.4156</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>9846.9719000000005</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>10169.597</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>10146.206099999999</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>10692.906499999999</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>10476.077499999999</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>10623.579100000001</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>10714.480799999999</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>11035.385399999999</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>10892.0412</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>11203.332</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>11760.774100000001</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>11656.4126</c:v>
+                </c:pt>
+                <c:pt idx="47" formatCode="General">
+                  <c:v>12115.6744</c:v>
+                </c:pt>
+                <c:pt idx="48" formatCode="General">
+                  <c:v>11797.9475</c:v>
+                </c:pt>
+                <c:pt idx="49" formatCode="General">
+                  <c:v>12618.302</c:v>
+                </c:pt>
+                <c:pt idx="50" formatCode="General">
+                  <c:v>13340.3681</c:v>
+                </c:pt>
+                <c:pt idx="51" formatCode="General">
+                  <c:v>14289.193799999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-6A80-46A0-99E3-3B20F67D5A48}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="595792384"/>
+        <c:axId val="595792056"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="595792384"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="595792056"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="595792056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="22500"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="595792384"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="2500"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -8283,6 +11182,46 @@
 </file>
 
 <file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -10386,6 +13325,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -10536,6 +13991,49 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5FDA04AE-34C2-4120-8381-6DF547C87E43}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B52DEEB-6CD3-4464-8BCD-45F08C2F449D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -22788,6 +26286,21 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA99CD91-F974-410B-85F4-1364969869DA}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V2" sqref="V2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D22590B1-852A-408F-A89B-FDBEE5F4FB6A}">
   <dimension ref="A1:D49"/>
@@ -24991,10 +28504,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6668C7CB-B2D1-4317-91E6-453829098F72}">
-  <dimension ref="A1:BB30"/>
+  <dimension ref="A1:BB31"/>
   <sheetViews>
-    <sheetView topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28748,6 +32261,199 @@
       </c>
       <c r="AW30" s="14"/>
     </row>
+    <row r="31" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" s="7">
+        <f>B23-B30</f>
+        <v>12431</v>
+      </c>
+      <c r="C31" s="7">
+        <f t="shared" ref="C31:AV31" si="4">C23-C30</f>
+        <v>12139</v>
+      </c>
+      <c r="D31" s="7">
+        <f t="shared" si="4"/>
+        <v>11746</v>
+      </c>
+      <c r="E31" s="7">
+        <f t="shared" si="4"/>
+        <v>10914</v>
+      </c>
+      <c r="F31" s="7">
+        <f t="shared" si="4"/>
+        <v>11093</v>
+      </c>
+      <c r="G31" s="7">
+        <f t="shared" si="4"/>
+        <v>10709</v>
+      </c>
+      <c r="H31" s="7">
+        <f t="shared" si="4"/>
+        <v>10877</v>
+      </c>
+      <c r="I31" s="7">
+        <f t="shared" si="4"/>
+        <v>10795</v>
+      </c>
+      <c r="J31" s="7">
+        <f t="shared" si="4"/>
+        <v>10646</v>
+      </c>
+      <c r="K31" s="7">
+        <f t="shared" si="4"/>
+        <v>10978</v>
+      </c>
+      <c r="L31" s="7">
+        <f t="shared" si="4"/>
+        <v>10790</v>
+      </c>
+      <c r="M31" s="7">
+        <f t="shared" si="4"/>
+        <v>10997</v>
+      </c>
+      <c r="N31" s="7">
+        <f t="shared" si="4"/>
+        <v>11905</v>
+      </c>
+      <c r="O31" s="7">
+        <f t="shared" si="4"/>
+        <v>12707</v>
+      </c>
+      <c r="P31" s="7">
+        <f t="shared" si="4"/>
+        <v>13786</v>
+      </c>
+      <c r="Q31" s="7">
+        <f t="shared" si="4"/>
+        <v>12600</v>
+      </c>
+      <c r="R31" s="7">
+        <f t="shared" si="4"/>
+        <v>11748</v>
+      </c>
+      <c r="S31" s="7">
+        <f t="shared" si="4"/>
+        <v>10606</v>
+      </c>
+      <c r="T31" s="7">
+        <f t="shared" si="4"/>
+        <v>9723</v>
+      </c>
+      <c r="U31" s="7">
+        <f t="shared" si="4"/>
+        <v>9086</v>
+      </c>
+      <c r="V31" s="7">
+        <f t="shared" si="4"/>
+        <v>9070</v>
+      </c>
+      <c r="W31" s="7">
+        <f t="shared" si="4"/>
+        <v>8439</v>
+      </c>
+      <c r="X31" s="7">
+        <f t="shared" si="4"/>
+        <v>8665</v>
+      </c>
+      <c r="Y31" s="7">
+        <f t="shared" si="4"/>
+        <v>8512</v>
+      </c>
+      <c r="Z31" s="7">
+        <f t="shared" si="4"/>
+        <v>8542</v>
+      </c>
+      <c r="AA31" s="7">
+        <f t="shared" si="4"/>
+        <v>9083</v>
+      </c>
+      <c r="AB31" s="7">
+        <f t="shared" si="4"/>
+        <v>8321</v>
+      </c>
+      <c r="AC31" s="7">
+        <f t="shared" si="4"/>
+        <v>8346</v>
+      </c>
+      <c r="AD31" s="7">
+        <f t="shared" si="4"/>
+        <v>8674</v>
+      </c>
+      <c r="AE31" s="7">
+        <f t="shared" si="4"/>
+        <v>8897</v>
+      </c>
+      <c r="AF31" s="7">
+        <f t="shared" si="4"/>
+        <v>8711</v>
+      </c>
+      <c r="AG31" s="7">
+        <f t="shared" si="4"/>
+        <v>8876</v>
+      </c>
+      <c r="AH31" s="7">
+        <f t="shared" si="4"/>
+        <v>10013</v>
+      </c>
+      <c r="AI31" s="7">
+        <f t="shared" si="4"/>
+        <v>8739</v>
+      </c>
+      <c r="AJ31" s="7">
+        <f t="shared" si="4"/>
+        <v>8583</v>
+      </c>
+      <c r="AK31" s="7">
+        <f t="shared" si="4"/>
+        <v>8984</v>
+      </c>
+      <c r="AL31" s="7">
+        <f t="shared" si="4"/>
+        <v>9040</v>
+      </c>
+      <c r="AM31" s="7">
+        <f t="shared" si="4"/>
+        <v>9292</v>
+      </c>
+      <c r="AN31" s="7">
+        <f t="shared" si="4"/>
+        <v>9361</v>
+      </c>
+      <c r="AO31" s="7">
+        <f t="shared" si="4"/>
+        <v>9612</v>
+      </c>
+      <c r="AP31" s="7">
+        <f t="shared" si="4"/>
+        <v>9825</v>
+      </c>
+      <c r="AQ31" s="7">
+        <f t="shared" si="4"/>
+        <v>9618</v>
+      </c>
+      <c r="AR31" s="7">
+        <f t="shared" si="4"/>
+        <v>9829</v>
+      </c>
+      <c r="AS31" s="7">
+        <f t="shared" si="4"/>
+        <v>9777</v>
+      </c>
+      <c r="AT31" s="7">
+        <f t="shared" si="4"/>
+        <v>9602</v>
+      </c>
+      <c r="AU31" s="7">
+        <f t="shared" si="4"/>
+        <v>9883</v>
+      </c>
+      <c r="AV31" s="7">
+        <f t="shared" si="4"/>
+        <v>10017</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -28802,7 +32508,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{909EECC5-39A5-4BE0-93C2-7E52FFE2180E}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="V15" sqref="V15"/>
     </sheetView>
   </sheetViews>

</xml_diff>